<commit_message>
added surrogate mutation function
</commit_message>
<xml_diff>
--- a/PAYE Analysis_5%Pension.xlsx
+++ b/PAYE Analysis_5%Pension.xlsx
@@ -371,7 +371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G191"/>
+  <dimension ref="A1:G192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4772,6 +4772,29 @@
         <v>9213.725</v>
       </c>
     </row>
+    <row r="192" spans="1:7">
+      <c r="A192" t="n">
+        <v>200000</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C192" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D192" t="n">
+        <v>7332.8</v>
+      </c>
+      <c r="E192" t="n">
+        <v>71600</v>
+      </c>
+      <c r="F192" t="n">
+        <v>111067.2</v>
+      </c>
+      <c r="G192" t="n">
+        <v>9255.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>